<commit_message>
Fix excel export layout, name display, vision fields
</commit_message>
<xml_diff>
--- a/templates/excel/입사지원서.xlsx
+++ b/templates/excel/입사지원서.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d16d419a79d4019c/dev/Humetix_Project/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{D6DA580A-CC61-4BB7-B199-D8C038C296A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36E9156A-080F-43D7-A583-B7B26C35230F}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{D6DA580A-CC61-4BB7-B199-D8C038C296A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D13AB22B-3650-49DE-A01D-77A21BA64D24}"/>
   <bookViews>
-    <workbookView xWindow="28650" yWindow="0" windowWidth="37755" windowHeight="21000" xr2:uid="{5B50BEF5-311F-42AB-98EF-5572324690B7}"/>
+    <workbookView xWindow="28410" yWindow="0" windowWidth="25590" windowHeight="21000" xr2:uid="{5B50BEF5-311F-42AB-98EF-5572324690B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="영진02-13김한결 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="날짜 이름" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'영진02-13김한결 (2)'!$A$1:$AR$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'날짜 이름'!$A$1:$AR$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1160,18 +1160,327 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1220,12 +1529,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center" indent="1"/>
     </xf>
@@ -1322,15 +1625,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1339,15 +1633,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1360,291 +1645,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2042,7 +2042,7 @@
   <dimension ref="A1:CC47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:U32"/>
+      <selection activeCell="BH14" sqref="BH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2084,67 +2084,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="24"/>
-      <c r="AS1" s="24"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="129"/>
+      <c r="Q1" s="129"/>
+      <c r="R1" s="129"/>
+      <c r="S1" s="129"/>
+      <c r="T1" s="129"/>
+      <c r="U1" s="129"/>
+      <c r="V1" s="129"/>
+      <c r="W1" s="129"/>
+      <c r="X1" s="129"/>
+      <c r="Y1" s="129"/>
+      <c r="Z1" s="129"/>
+      <c r="AA1" s="129"/>
+      <c r="AB1" s="129"/>
+      <c r="AC1" s="129"/>
+      <c r="AD1" s="129"/>
+      <c r="AE1" s="129"/>
+      <c r="AF1" s="129"/>
+      <c r="AG1" s="129"/>
+      <c r="AH1" s="129"/>
+      <c r="AI1" s="129"/>
+      <c r="AJ1" s="129"/>
+      <c r="AK1" s="129"/>
+      <c r="AL1" s="129"/>
+      <c r="AM1" s="129"/>
+      <c r="AN1" s="129"/>
+      <c r="AO1" s="129"/>
+      <c r="AP1" s="129"/>
+      <c r="AQ1" s="129"/>
+      <c r="AR1" s="129"/>
+      <c r="AS1" s="129"/>
     </row>
     <row r="2" spans="1:45" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="133"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -2180,18 +2180,18 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:45" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="36"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="139"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
@@ -2209,432 +2209,432 @@
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
       <c r="AB3" s="9"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="37"/>
-      <c r="AQ3" s="37"/>
-      <c r="AR3" s="37"/>
+      <c r="AC3" s="140"/>
+      <c r="AD3" s="140"/>
+      <c r="AE3" s="140"/>
+      <c r="AF3" s="140"/>
+      <c r="AG3" s="140"/>
+      <c r="AH3" s="140"/>
+      <c r="AI3" s="140"/>
+      <c r="AJ3" s="140"/>
+      <c r="AK3" s="140"/>
+      <c r="AL3" s="140"/>
+      <c r="AM3" s="140"/>
+      <c r="AN3" s="140"/>
+      <c r="AO3" s="140"/>
+      <c r="AP3" s="140"/>
+      <c r="AQ3" s="140"/>
+      <c r="AR3" s="140"/>
     </row>
     <row r="4" spans="1:45" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="58" t="s">
+      <c r="B4" s="150"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="64" t="s">
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="161"/>
+      <c r="O4" s="165" t="s">
         <v>90</v>
       </c>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="65"/>
-      <c r="Z4" s="65"/>
-      <c r="AA4" s="65"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="67" t="s">
+      <c r="P4" s="166"/>
+      <c r="Q4" s="166"/>
+      <c r="R4" s="166"/>
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="166"/>
+      <c r="Y4" s="166"/>
+      <c r="Z4" s="166"/>
+      <c r="AA4" s="166"/>
+      <c r="AB4" s="167"/>
+      <c r="AC4" s="168" t="s">
         <v>4</v>
       </c>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59"/>
-      <c r="AF4" s="60"/>
-      <c r="AG4" s="69" t="s">
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="160"/>
+      <c r="AF4" s="161"/>
+      <c r="AG4" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="AH4" s="70"/>
-      <c r="AI4" s="70"/>
-      <c r="AJ4" s="70"/>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="70"/>
-      <c r="AN4" s="70"/>
-      <c r="AO4" s="70"/>
-      <c r="AP4" s="70"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="71"/>
+      <c r="AH4" s="171"/>
+      <c r="AI4" s="171"/>
+      <c r="AJ4" s="171"/>
+      <c r="AK4" s="171"/>
+      <c r="AL4" s="171"/>
+      <c r="AM4" s="171"/>
+      <c r="AN4" s="171"/>
+      <c r="AO4" s="171"/>
+      <c r="AP4" s="171"/>
+      <c r="AQ4" s="171"/>
+      <c r="AR4" s="172"/>
     </row>
     <row r="5" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="52"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="75" t="s">
+      <c r="B5" s="153"/>
+      <c r="C5" s="154"/>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="162"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="164"/>
+      <c r="O5" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="76"/>
-      <c r="U5" s="76"/>
-      <c r="V5" s="76"/>
-      <c r="W5" s="76"/>
-      <c r="X5" s="76"/>
-      <c r="Y5" s="76"/>
-      <c r="Z5" s="76"/>
-      <c r="AA5" s="76"/>
-      <c r="AB5" s="77"/>
-      <c r="AC5" s="68"/>
-      <c r="AD5" s="62"/>
-      <c r="AE5" s="62"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="72"/>
-      <c r="AH5" s="73"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="73"/>
-      <c r="AK5" s="73"/>
-      <c r="AL5" s="73"/>
-      <c r="AM5" s="73"/>
-      <c r="AN5" s="73"/>
-      <c r="AO5" s="73"/>
-      <c r="AP5" s="73"/>
-      <c r="AQ5" s="73"/>
-      <c r="AR5" s="74"/>
+      <c r="P5" s="177"/>
+      <c r="Q5" s="177"/>
+      <c r="R5" s="177"/>
+      <c r="S5" s="177"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="W5" s="177"/>
+      <c r="X5" s="177"/>
+      <c r="Y5" s="177"/>
+      <c r="Z5" s="177"/>
+      <c r="AA5" s="177"/>
+      <c r="AB5" s="178"/>
+      <c r="AC5" s="169"/>
+      <c r="AD5" s="163"/>
+      <c r="AE5" s="163"/>
+      <c r="AF5" s="164"/>
+      <c r="AG5" s="173"/>
+      <c r="AH5" s="174"/>
+      <c r="AI5" s="174"/>
+      <c r="AJ5" s="174"/>
+      <c r="AK5" s="174"/>
+      <c r="AL5" s="174"/>
+      <c r="AM5" s="174"/>
+      <c r="AN5" s="174"/>
+      <c r="AO5" s="174"/>
+      <c r="AP5" s="174"/>
+      <c r="AQ5" s="174"/>
+      <c r="AR5" s="175"/>
     </row>
     <row r="6" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="78" t="s">
+      <c r="B6" s="153"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="154"/>
+      <c r="G6" s="154"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="81" t="s">
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="179" t="s">
         <v>91</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
-      <c r="X6" s="82"/>
-      <c r="Y6" s="82"/>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="83"/>
-      <c r="AC6" s="84" t="s">
+      <c r="P6" s="180"/>
+      <c r="Q6" s="180"/>
+      <c r="R6" s="180"/>
+      <c r="S6" s="180"/>
+      <c r="T6" s="180"/>
+      <c r="U6" s="180"/>
+      <c r="V6" s="180"/>
+      <c r="W6" s="180"/>
+      <c r="X6" s="180"/>
+      <c r="Y6" s="180"/>
+      <c r="Z6" s="180"/>
+      <c r="AA6" s="180"/>
+      <c r="AB6" s="181"/>
+      <c r="AC6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AD6" s="85"/>
-      <c r="AE6" s="85"/>
-      <c r="AF6" s="86"/>
-      <c r="AG6" s="81" t="s">
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="40"/>
+      <c r="AG6" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="AH6" s="82"/>
-      <c r="AI6" s="82"/>
-      <c r="AJ6" s="82"/>
-      <c r="AK6" s="82"/>
-      <c r="AL6" s="82"/>
-      <c r="AM6" s="82"/>
-      <c r="AN6" s="82"/>
-      <c r="AO6" s="82"/>
-      <c r="AP6" s="82"/>
-      <c r="AQ6" s="82"/>
-      <c r="AR6" s="87"/>
+      <c r="AH6" s="180"/>
+      <c r="AI6" s="180"/>
+      <c r="AJ6" s="180"/>
+      <c r="AK6" s="180"/>
+      <c r="AL6" s="180"/>
+      <c r="AM6" s="180"/>
+      <c r="AN6" s="180"/>
+      <c r="AO6" s="180"/>
+      <c r="AP6" s="180"/>
+      <c r="AQ6" s="180"/>
+      <c r="AR6" s="182"/>
     </row>
     <row r="7" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="78" t="s">
+      <c r="B7" s="153"/>
+      <c r="C7" s="154"/>
+      <c r="D7" s="154"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="154"/>
+      <c r="G7" s="154"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="106"/>
-      <c r="W7" s="106"/>
-      <c r="X7" s="106"/>
-      <c r="Y7" s="106"/>
-      <c r="Z7" s="106"/>
-      <c r="AA7" s="106"/>
-      <c r="AB7" s="106"/>
-      <c r="AC7" s="106"/>
-      <c r="AD7" s="106"/>
-      <c r="AE7" s="106"/>
-      <c r="AF7" s="106"/>
-      <c r="AG7" s="106"/>
-      <c r="AH7" s="106"/>
-      <c r="AI7" s="106"/>
-      <c r="AJ7" s="106"/>
-      <c r="AK7" s="106"/>
-      <c r="AL7" s="106"/>
-      <c r="AM7" s="106"/>
-      <c r="AN7" s="106"/>
-      <c r="AO7" s="106"/>
-      <c r="AP7" s="106"/>
-      <c r="AQ7" s="106"/>
-      <c r="AR7" s="107"/>
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="122"/>
+      <c r="P7" s="123"/>
+      <c r="Q7" s="123"/>
+      <c r="R7" s="123"/>
+      <c r="S7" s="123"/>
+      <c r="T7" s="123"/>
+      <c r="U7" s="123"/>
+      <c r="V7" s="123"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="123"/>
+      <c r="AB7" s="123"/>
+      <c r="AC7" s="123"/>
+      <c r="AD7" s="123"/>
+      <c r="AE7" s="123"/>
+      <c r="AF7" s="123"/>
+      <c r="AG7" s="123"/>
+      <c r="AH7" s="123"/>
+      <c r="AI7" s="123"/>
+      <c r="AJ7" s="123"/>
+      <c r="AK7" s="123"/>
+      <c r="AL7" s="123"/>
+      <c r="AM7" s="123"/>
+      <c r="AN7" s="123"/>
+      <c r="AO7" s="123"/>
+      <c r="AP7" s="123"/>
+      <c r="AQ7" s="123"/>
+      <c r="AR7" s="124"/>
     </row>
     <row r="8" spans="1:45" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="55"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="108" t="s">
+      <c r="B8" s="156"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="157"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="111" t="s">
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="112"/>
-      <c r="Q8" s="112"/>
-      <c r="R8" s="112"/>
-      <c r="S8" s="112"/>
-      <c r="T8" s="112"/>
-      <c r="U8" s="112"/>
-      <c r="V8" s="112"/>
-      <c r="W8" s="112"/>
-      <c r="X8" s="112"/>
-      <c r="Y8" s="112"/>
-      <c r="Z8" s="112"/>
-      <c r="AA8" s="112"/>
-      <c r="AB8" s="112"/>
-      <c r="AC8" s="112"/>
-      <c r="AD8" s="112"/>
-      <c r="AE8" s="112"/>
-      <c r="AF8" s="112"/>
-      <c r="AG8" s="112"/>
-      <c r="AH8" s="112"/>
-      <c r="AI8" s="112"/>
-      <c r="AJ8" s="112"/>
-      <c r="AK8" s="112"/>
-      <c r="AL8" s="112"/>
-      <c r="AM8" s="112"/>
-      <c r="AN8" s="112"/>
-      <c r="AO8" s="112"/>
-      <c r="AP8" s="112"/>
-      <c r="AQ8" s="112"/>
-      <c r="AR8" s="113"/>
+      <c r="P8" s="127"/>
+      <c r="Q8" s="127"/>
+      <c r="R8" s="127"/>
+      <c r="S8" s="127"/>
+      <c r="T8" s="127"/>
+      <c r="U8" s="127"/>
+      <c r="V8" s="127"/>
+      <c r="W8" s="127"/>
+      <c r="X8" s="127"/>
+      <c r="Y8" s="127"/>
+      <c r="Z8" s="127"/>
+      <c r="AA8" s="127"/>
+      <c r="AB8" s="127"/>
+      <c r="AC8" s="127"/>
+      <c r="AD8" s="127"/>
+      <c r="AE8" s="127"/>
+      <c r="AF8" s="127"/>
+      <c r="AG8" s="127"/>
+      <c r="AH8" s="127"/>
+      <c r="AI8" s="127"/>
+      <c r="AJ8" s="127"/>
+      <c r="AK8" s="127"/>
+      <c r="AL8" s="127"/>
+      <c r="AM8" s="127"/>
+      <c r="AN8" s="127"/>
+      <c r="AO8" s="127"/>
+      <c r="AP8" s="127"/>
+      <c r="AQ8" s="127"/>
+      <c r="AR8" s="128"/>
       <c r="AS8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:45" ht="9.9499999999999993" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:45" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="44" t="s">
+      <c r="C10" s="142"/>
+      <c r="D10" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="44" t="s">
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="44" t="s">
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="76"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="76"/>
+      <c r="V10" s="76"/>
+      <c r="W10" s="76"/>
+      <c r="X10" s="76"/>
+      <c r="Y10" s="76"/>
+      <c r="Z10" s="76"/>
+      <c r="AA10" s="76"/>
+      <c r="AB10" s="77"/>
+      <c r="AC10" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="26"/>
-      <c r="AF10" s="26"/>
-      <c r="AG10" s="26"/>
-      <c r="AH10" s="26"/>
-      <c r="AI10" s="26"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="44" t="s">
+      <c r="AD10" s="76"/>
+      <c r="AE10" s="76"/>
+      <c r="AF10" s="76"/>
+      <c r="AG10" s="76"/>
+      <c r="AH10" s="76"/>
+      <c r="AI10" s="76"/>
+      <c r="AJ10" s="77"/>
+      <c r="AK10" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="AL10" s="26"/>
-      <c r="AM10" s="26"/>
-      <c r="AN10" s="26"/>
-      <c r="AO10" s="26"/>
-      <c r="AP10" s="26"/>
-      <c r="AQ10" s="26"/>
-      <c r="AR10" s="45"/>
+      <c r="AL10" s="76"/>
+      <c r="AM10" s="76"/>
+      <c r="AN10" s="76"/>
+      <c r="AO10" s="76"/>
+      <c r="AP10" s="76"/>
+      <c r="AQ10" s="76"/>
+      <c r="AR10" s="81"/>
     </row>
     <row r="11" spans="1:45" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="46" t="s">
+      <c r="B11" s="143"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="88" t="s">
+      <c r="E11" s="148"/>
+      <c r="F11" s="148"/>
+      <c r="G11" s="148"/>
+      <c r="H11" s="148"/>
+      <c r="I11" s="148"/>
+      <c r="J11" s="148"/>
+      <c r="K11" s="148"/>
+      <c r="L11" s="148"/>
+      <c r="M11" s="148"/>
+      <c r="N11" s="149"/>
+      <c r="O11" s="183" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
-      <c r="S11" s="89"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="89"/>
-      <c r="V11" s="89"/>
-      <c r="W11" s="89"/>
-      <c r="X11" s="89"/>
-      <c r="Y11" s="89"/>
-      <c r="Z11" s="89"/>
-      <c r="AA11" s="89"/>
-      <c r="AB11" s="90"/>
-      <c r="AC11" s="91"/>
-      <c r="AD11" s="92"/>
-      <c r="AE11" s="92"/>
-      <c r="AF11" s="92"/>
-      <c r="AG11" s="92"/>
-      <c r="AH11" s="92"/>
-      <c r="AI11" s="92"/>
-      <c r="AJ11" s="93"/>
-      <c r="AK11" s="91" t="s">
+      <c r="P11" s="184"/>
+      <c r="Q11" s="184"/>
+      <c r="R11" s="184"/>
+      <c r="S11" s="184"/>
+      <c r="T11" s="184"/>
+      <c r="U11" s="184"/>
+      <c r="V11" s="184"/>
+      <c r="W11" s="184"/>
+      <c r="X11" s="184"/>
+      <c r="Y11" s="184"/>
+      <c r="Z11" s="184"/>
+      <c r="AA11" s="184"/>
+      <c r="AB11" s="185"/>
+      <c r="AC11" s="35"/>
+      <c r="AD11" s="36"/>
+      <c r="AE11" s="36"/>
+      <c r="AF11" s="36"/>
+      <c r="AG11" s="36"/>
+      <c r="AH11" s="36"/>
+      <c r="AI11" s="36"/>
+      <c r="AJ11" s="37"/>
+      <c r="AK11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="AL11" s="92"/>
-      <c r="AM11" s="92"/>
-      <c r="AN11" s="92"/>
-      <c r="AO11" s="92"/>
-      <c r="AP11" s="92"/>
-      <c r="AQ11" s="92"/>
-      <c r="AR11" s="94"/>
+      <c r="AL11" s="36"/>
+      <c r="AM11" s="36"/>
+      <c r="AN11" s="36"/>
+      <c r="AO11" s="36"/>
+      <c r="AP11" s="36"/>
+      <c r="AQ11" s="36"/>
+      <c r="AR11" s="100"/>
     </row>
     <row r="12" spans="1:45" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="95" t="s">
+      <c r="B12" s="145"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="96"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="96"/>
-      <c r="M12" s="96"/>
-      <c r="N12" s="97"/>
-      <c r="O12" s="98" t="s">
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="99"/>
-      <c r="Q12" s="99"/>
-      <c r="R12" s="99"/>
-      <c r="S12" s="99"/>
-      <c r="T12" s="99"/>
-      <c r="U12" s="99"/>
-      <c r="V12" s="99"/>
-      <c r="W12" s="99"/>
-      <c r="X12" s="99"/>
-      <c r="Y12" s="99"/>
-      <c r="Z12" s="99"/>
-      <c r="AA12" s="99"/>
-      <c r="AB12" s="100"/>
-      <c r="AC12" s="101"/>
-      <c r="AD12" s="102"/>
-      <c r="AE12" s="102"/>
-      <c r="AF12" s="102"/>
-      <c r="AG12" s="102"/>
-      <c r="AH12" s="102"/>
-      <c r="AI12" s="102"/>
-      <c r="AJ12" s="103"/>
-      <c r="AK12" s="101" t="s">
+      <c r="P12" s="117"/>
+      <c r="Q12" s="117"/>
+      <c r="R12" s="117"/>
+      <c r="S12" s="117"/>
+      <c r="T12" s="117"/>
+      <c r="U12" s="117"/>
+      <c r="V12" s="117"/>
+      <c r="W12" s="117"/>
+      <c r="X12" s="117"/>
+      <c r="Y12" s="117"/>
+      <c r="Z12" s="117"/>
+      <c r="AA12" s="117"/>
+      <c r="AB12" s="118"/>
+      <c r="AC12" s="44"/>
+      <c r="AD12" s="45"/>
+      <c r="AE12" s="45"/>
+      <c r="AF12" s="45"/>
+      <c r="AG12" s="45"/>
+      <c r="AH12" s="45"/>
+      <c r="AI12" s="45"/>
+      <c r="AJ12" s="46"/>
+      <c r="AK12" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="AL12" s="102"/>
-      <c r="AM12" s="102"/>
-      <c r="AN12" s="102"/>
-      <c r="AO12" s="102"/>
-      <c r="AP12" s="102"/>
-      <c r="AQ12" s="102"/>
-      <c r="AR12" s="104"/>
+      <c r="AL12" s="45"/>
+      <c r="AM12" s="45"/>
+      <c r="AN12" s="45"/>
+      <c r="AO12" s="45"/>
+      <c r="AP12" s="45"/>
+      <c r="AQ12" s="45"/>
+      <c r="AR12" s="73"/>
     </row>
     <row r="13" spans="1:45" ht="9.9499999999999993" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9"/>
@@ -2682,218 +2682,218 @@
       <c r="AR13" s="9"/>
     </row>
     <row r="14" spans="1:45" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="126" t="s">
+      <c r="B14" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="44" t="s">
+      <c r="C14" s="108"/>
+      <c r="D14" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="44" t="s">
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="44" t="s">
+      <c r="P14" s="76"/>
+      <c r="Q14" s="76"/>
+      <c r="R14" s="76"/>
+      <c r="S14" s="76"/>
+      <c r="T14" s="76"/>
+      <c r="U14" s="76"/>
+      <c r="V14" s="76"/>
+      <c r="W14" s="76"/>
+      <c r="X14" s="76"/>
+      <c r="Y14" s="76"/>
+      <c r="Z14" s="76"/>
+      <c r="AA14" s="76"/>
+      <c r="AB14" s="77"/>
+      <c r="AC14" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="AD14" s="26"/>
-      <c r="AE14" s="26"/>
-      <c r="AF14" s="26"/>
-      <c r="AG14" s="26"/>
-      <c r="AH14" s="26"/>
-      <c r="AI14" s="26"/>
-      <c r="AJ14" s="27"/>
-      <c r="AK14" s="44" t="s">
+      <c r="AD14" s="76"/>
+      <c r="AE14" s="76"/>
+      <c r="AF14" s="76"/>
+      <c r="AG14" s="76"/>
+      <c r="AH14" s="76"/>
+      <c r="AI14" s="76"/>
+      <c r="AJ14" s="77"/>
+      <c r="AK14" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="AL14" s="26"/>
-      <c r="AM14" s="26"/>
-      <c r="AN14" s="26"/>
-      <c r="AO14" s="26"/>
-      <c r="AP14" s="26"/>
-      <c r="AQ14" s="26"/>
-      <c r="AR14" s="45"/>
+      <c r="AL14" s="76"/>
+      <c r="AM14" s="76"/>
+      <c r="AN14" s="76"/>
+      <c r="AO14" s="76"/>
+      <c r="AP14" s="76"/>
+      <c r="AQ14" s="76"/>
+      <c r="AR14" s="81"/>
     </row>
     <row r="15" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="128"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="132" t="s">
+      <c r="B15" s="109"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="133"/>
-      <c r="F15" s="133"/>
-      <c r="G15" s="133"/>
-      <c r="H15" s="133"/>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
-      <c r="K15" s="133"/>
-      <c r="L15" s="133"/>
-      <c r="M15" s="133"/>
-      <c r="N15" s="134"/>
-      <c r="O15" s="114" t="s">
+      <c r="E15" s="114"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="N15" s="115"/>
+      <c r="O15" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="P15" s="115"/>
-      <c r="Q15" s="115"/>
-      <c r="R15" s="115"/>
-      <c r="S15" s="115"/>
-      <c r="T15" s="115"/>
-      <c r="U15" s="115"/>
-      <c r="V15" s="115"/>
-      <c r="W15" s="115"/>
-      <c r="X15" s="115"/>
-      <c r="Y15" s="115"/>
-      <c r="Z15" s="115"/>
-      <c r="AA15" s="115"/>
-      <c r="AB15" s="116"/>
-      <c r="AC15" s="117" t="s">
+      <c r="P15" s="95"/>
+      <c r="Q15" s="95"/>
+      <c r="R15" s="95"/>
+      <c r="S15" s="95"/>
+      <c r="T15" s="95"/>
+      <c r="U15" s="95"/>
+      <c r="V15" s="95"/>
+      <c r="W15" s="95"/>
+      <c r="X15" s="95"/>
+      <c r="Y15" s="95"/>
+      <c r="Z15" s="95"/>
+      <c r="AA15" s="95"/>
+      <c r="AB15" s="96"/>
+      <c r="AC15" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="AD15" s="118"/>
-      <c r="AE15" s="118"/>
-      <c r="AF15" s="118"/>
-      <c r="AG15" s="118"/>
-      <c r="AH15" s="118"/>
-      <c r="AI15" s="118"/>
-      <c r="AJ15" s="119"/>
-      <c r="AK15" s="91" t="s">
+      <c r="AD15" s="98"/>
+      <c r="AE15" s="98"/>
+      <c r="AF15" s="98"/>
+      <c r="AG15" s="98"/>
+      <c r="AH15" s="98"/>
+      <c r="AI15" s="98"/>
+      <c r="AJ15" s="99"/>
+      <c r="AK15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="AL15" s="92"/>
-      <c r="AM15" s="92"/>
-      <c r="AN15" s="92"/>
-      <c r="AO15" s="92"/>
-      <c r="AP15" s="92"/>
-      <c r="AQ15" s="92"/>
-      <c r="AR15" s="94"/>
+      <c r="AL15" s="36"/>
+      <c r="AM15" s="36"/>
+      <c r="AN15" s="36"/>
+      <c r="AO15" s="36"/>
+      <c r="AP15" s="36"/>
+      <c r="AQ15" s="36"/>
+      <c r="AR15" s="100"/>
     </row>
     <row r="16" spans="1:45" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="128"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="91" t="s">
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="92"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="114" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="P16" s="115"/>
-      <c r="Q16" s="115"/>
-      <c r="R16" s="115"/>
-      <c r="S16" s="115"/>
-      <c r="T16" s="115"/>
-      <c r="U16" s="115"/>
-      <c r="V16" s="115"/>
-      <c r="W16" s="115"/>
-      <c r="X16" s="115"/>
-      <c r="Y16" s="115"/>
-      <c r="Z16" s="115"/>
-      <c r="AA16" s="115"/>
-      <c r="AB16" s="116"/>
-      <c r="AC16" s="117" t="s">
+      <c r="P16" s="95"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="95"/>
+      <c r="T16" s="95"/>
+      <c r="U16" s="95"/>
+      <c r="V16" s="95"/>
+      <c r="W16" s="95"/>
+      <c r="X16" s="95"/>
+      <c r="Y16" s="95"/>
+      <c r="Z16" s="95"/>
+      <c r="AA16" s="95"/>
+      <c r="AB16" s="96"/>
+      <c r="AC16" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="AD16" s="118"/>
-      <c r="AE16" s="118"/>
-      <c r="AF16" s="118"/>
-      <c r="AG16" s="118"/>
-      <c r="AH16" s="118"/>
-      <c r="AI16" s="118"/>
-      <c r="AJ16" s="119"/>
-      <c r="AK16" s="91" t="s">
+      <c r="AD16" s="98"/>
+      <c r="AE16" s="98"/>
+      <c r="AF16" s="98"/>
+      <c r="AG16" s="98"/>
+      <c r="AH16" s="98"/>
+      <c r="AI16" s="98"/>
+      <c r="AJ16" s="99"/>
+      <c r="AK16" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="AL16" s="92"/>
-      <c r="AM16" s="92"/>
-      <c r="AN16" s="92"/>
-      <c r="AO16" s="92"/>
-      <c r="AP16" s="92"/>
-      <c r="AQ16" s="92"/>
-      <c r="AR16" s="94"/>
+      <c r="AL16" s="36"/>
+      <c r="AM16" s="36"/>
+      <c r="AN16" s="36"/>
+      <c r="AO16" s="36"/>
+      <c r="AP16" s="36"/>
+      <c r="AQ16" s="36"/>
+      <c r="AR16" s="100"/>
     </row>
     <row r="17" spans="2:60" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="130"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="101" t="s">
+      <c r="B17" s="111"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="102"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="103"/>
-      <c r="O17" s="120" t="s">
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="121"/>
-      <c r="Q17" s="121"/>
-      <c r="R17" s="121"/>
-      <c r="S17" s="121"/>
-      <c r="T17" s="121"/>
-      <c r="U17" s="121"/>
-      <c r="V17" s="121"/>
-      <c r="W17" s="121"/>
-      <c r="X17" s="121"/>
-      <c r="Y17" s="121"/>
-      <c r="Z17" s="121"/>
-      <c r="AA17" s="121"/>
-      <c r="AB17" s="122"/>
-      <c r="AC17" s="123" t="s">
+      <c r="P17" s="102"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="102"/>
+      <c r="T17" s="102"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="102"/>
+      <c r="W17" s="102"/>
+      <c r="X17" s="102"/>
+      <c r="Y17" s="102"/>
+      <c r="Z17" s="102"/>
+      <c r="AA17" s="102"/>
+      <c r="AB17" s="103"/>
+      <c r="AC17" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="AD17" s="124"/>
-      <c r="AE17" s="124"/>
-      <c r="AF17" s="124"/>
-      <c r="AG17" s="124"/>
-      <c r="AH17" s="124"/>
-      <c r="AI17" s="124"/>
-      <c r="AJ17" s="125"/>
-      <c r="AK17" s="101" t="s">
+      <c r="AD17" s="105"/>
+      <c r="AE17" s="105"/>
+      <c r="AF17" s="105"/>
+      <c r="AG17" s="105"/>
+      <c r="AH17" s="105"/>
+      <c r="AI17" s="105"/>
+      <c r="AJ17" s="106"/>
+      <c r="AK17" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="AL17" s="102"/>
-      <c r="AM17" s="102"/>
-      <c r="AN17" s="102"/>
-      <c r="AO17" s="102"/>
-      <c r="AP17" s="102"/>
-      <c r="AQ17" s="102"/>
-      <c r="AR17" s="104"/>
+      <c r="AL17" s="45"/>
+      <c r="AM17" s="45"/>
+      <c r="AN17" s="45"/>
+      <c r="AO17" s="45"/>
+      <c r="AP17" s="45"/>
+      <c r="AQ17" s="45"/>
+      <c r="AR17" s="73"/>
     </row>
     <row r="18" spans="2:60" ht="9.9499999999999993" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
@@ -2941,108 +2941,108 @@
       <c r="AR18" s="9"/>
     </row>
     <row r="19" spans="2:60" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="135" t="s">
+      <c r="B19" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="136"/>
-      <c r="D19" s="44" t="s">
+      <c r="C19" s="55"/>
+      <c r="D19" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="44" t="s">
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="44" t="s">
+      <c r="L19" s="76"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="76"/>
+      <c r="O19" s="76"/>
+      <c r="P19" s="76"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="76"/>
+      <c r="S19" s="76"/>
+      <c r="T19" s="76"/>
+      <c r="U19" s="77"/>
+      <c r="V19" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="26"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="26"/>
-      <c r="AE19" s="26"/>
-      <c r="AF19" s="27"/>
-      <c r="AG19" s="44" t="s">
+      <c r="W19" s="76"/>
+      <c r="X19" s="76"/>
+      <c r="Y19" s="76"/>
+      <c r="Z19" s="76"/>
+      <c r="AA19" s="76"/>
+      <c r="AB19" s="76"/>
+      <c r="AC19" s="76"/>
+      <c r="AD19" s="76"/>
+      <c r="AE19" s="76"/>
+      <c r="AF19" s="77"/>
+      <c r="AG19" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="AH19" s="26"/>
-      <c r="AI19" s="26"/>
-      <c r="AJ19" s="26"/>
-      <c r="AK19" s="26"/>
-      <c r="AL19" s="26"/>
-      <c r="AM19" s="26"/>
-      <c r="AN19" s="26"/>
-      <c r="AO19" s="26"/>
-      <c r="AP19" s="26"/>
-      <c r="AQ19" s="26"/>
-      <c r="AR19" s="45"/>
+      <c r="AH19" s="76"/>
+      <c r="AI19" s="76"/>
+      <c r="AJ19" s="76"/>
+      <c r="AK19" s="76"/>
+      <c r="AL19" s="76"/>
+      <c r="AM19" s="76"/>
+      <c r="AN19" s="76"/>
+      <c r="AO19" s="76"/>
+      <c r="AP19" s="76"/>
+      <c r="AQ19" s="76"/>
+      <c r="AR19" s="81"/>
     </row>
     <row r="20" spans="2:60" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="137"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="101" t="s">
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="102"/>
-      <c r="J20" s="103"/>
-      <c r="K20" s="95" t="s">
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="96"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="96"/>
-      <c r="T20" s="96"/>
-      <c r="U20" s="97"/>
-      <c r="V20" s="101"/>
-      <c r="W20" s="102"/>
-      <c r="X20" s="102"/>
-      <c r="Y20" s="102"/>
-      <c r="Z20" s="102"/>
-      <c r="AA20" s="102"/>
-      <c r="AB20" s="102"/>
-      <c r="AC20" s="102"/>
-      <c r="AD20" s="102"/>
-      <c r="AE20" s="102"/>
-      <c r="AF20" s="103"/>
-      <c r="AG20" s="101"/>
-      <c r="AH20" s="102"/>
-      <c r="AI20" s="102"/>
-      <c r="AJ20" s="102"/>
-      <c r="AK20" s="102"/>
-      <c r="AL20" s="102"/>
-      <c r="AM20" s="102"/>
-      <c r="AN20" s="102"/>
-      <c r="AO20" s="102"/>
-      <c r="AP20" s="102"/>
-      <c r="AQ20" s="102"/>
-      <c r="AR20" s="104"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="92"/>
+      <c r="N20" s="92"/>
+      <c r="O20" s="92"/>
+      <c r="P20" s="92"/>
+      <c r="Q20" s="92"/>
+      <c r="R20" s="92"/>
+      <c r="S20" s="92"/>
+      <c r="T20" s="92"/>
+      <c r="U20" s="93"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="45"/>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="45"/>
+      <c r="AB20" s="45"/>
+      <c r="AC20" s="45"/>
+      <c r="AD20" s="45"/>
+      <c r="AE20" s="45"/>
+      <c r="AF20" s="46"/>
+      <c r="AG20" s="44"/>
+      <c r="AH20" s="45"/>
+      <c r="AI20" s="45"/>
+      <c r="AJ20" s="45"/>
+      <c r="AK20" s="45"/>
+      <c r="AL20" s="45"/>
+      <c r="AM20" s="45"/>
+      <c r="AN20" s="45"/>
+      <c r="AO20" s="45"/>
+      <c r="AP20" s="45"/>
+      <c r="AQ20" s="45"/>
+      <c r="AR20" s="73"/>
     </row>
     <row r="21" spans="2:60" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="9"/>
@@ -3090,130 +3090,130 @@
       <c r="AR21" s="9"/>
     </row>
     <row r="22" spans="2:60" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="135" t="s">
+      <c r="B22" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="145" t="s">
+      <c r="C22" s="55"/>
+      <c r="D22" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="147"/>
-      <c r="K22" s="44" t="s">
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="44" t="s">
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="77"/>
+      <c r="O22" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="44" t="s">
+      <c r="P22" s="76"/>
+      <c r="Q22" s="77"/>
+      <c r="R22" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="27"/>
-      <c r="AC22" s="44" t="s">
+      <c r="S22" s="76"/>
+      <c r="T22" s="76"/>
+      <c r="U22" s="76"/>
+      <c r="V22" s="76"/>
+      <c r="W22" s="76"/>
+      <c r="X22" s="76"/>
+      <c r="Y22" s="76"/>
+      <c r="Z22" s="76"/>
+      <c r="AA22" s="76"/>
+      <c r="AB22" s="77"/>
+      <c r="AC22" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="AD22" s="26"/>
-      <c r="AE22" s="26"/>
-      <c r="AF22" s="27"/>
-      <c r="AG22" s="44" t="s">
+      <c r="AD22" s="76"/>
+      <c r="AE22" s="76"/>
+      <c r="AF22" s="77"/>
+      <c r="AG22" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="AH22" s="26"/>
-      <c r="AI22" s="26"/>
-      <c r="AJ22" s="27"/>
-      <c r="AK22" s="44" t="s">
+      <c r="AH22" s="76"/>
+      <c r="AI22" s="76"/>
+      <c r="AJ22" s="77"/>
+      <c r="AK22" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="AL22" s="26"/>
-      <c r="AM22" s="26"/>
-      <c r="AN22" s="26"/>
-      <c r="AO22" s="27"/>
-      <c r="AP22" s="44" t="s">
+      <c r="AL22" s="76"/>
+      <c r="AM22" s="76"/>
+      <c r="AN22" s="76"/>
+      <c r="AO22" s="77"/>
+      <c r="AP22" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="AQ22" s="26"/>
-      <c r="AR22" s="45"/>
+      <c r="AQ22" s="76"/>
+      <c r="AR22" s="81"/>
     </row>
     <row r="23" spans="2:60" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="137"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="149"/>
-      <c r="F23" s="149"/>
-      <c r="G23" s="149"/>
-      <c r="H23" s="149"/>
-      <c r="I23" s="149"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="142" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="143"/>
-      <c r="M23" s="143"/>
-      <c r="N23" s="144"/>
-      <c r="O23" s="142" t="s">
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="84"/>
+      <c r="O23" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="P23" s="143"/>
-      <c r="Q23" s="144"/>
-      <c r="R23" s="101" t="s">
+      <c r="P23" s="83"/>
+      <c r="Q23" s="84"/>
+      <c r="R23" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="S23" s="102"/>
-      <c r="T23" s="102"/>
-      <c r="U23" s="102" t="s">
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="V23" s="102"/>
-      <c r="W23" s="102" t="s">
+      <c r="V23" s="45"/>
+      <c r="W23" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="X23" s="102"/>
-      <c r="Y23" s="102"/>
-      <c r="Z23" s="102" t="s">
+      <c r="X23" s="45"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="AA23" s="102"/>
-      <c r="AB23" s="103"/>
-      <c r="AC23" s="101" t="s">
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="AD23" s="102"/>
-      <c r="AE23" s="102"/>
-      <c r="AF23" s="103"/>
-      <c r="AG23" s="101" t="s">
+      <c r="AD23" s="45"/>
+      <c r="AE23" s="45"/>
+      <c r="AF23" s="46"/>
+      <c r="AG23" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="AH23" s="102"/>
-      <c r="AI23" s="102"/>
-      <c r="AJ23" s="103"/>
-      <c r="AK23" s="101" t="s">
+      <c r="AH23" s="45"/>
+      <c r="AI23" s="45"/>
+      <c r="AJ23" s="46"/>
+      <c r="AK23" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="AL23" s="102"/>
-      <c r="AM23" s="102"/>
-      <c r="AN23" s="102"/>
-      <c r="AO23" s="103"/>
-      <c r="AP23" s="101"/>
-      <c r="AQ23" s="102"/>
-      <c r="AR23" s="104"/>
+      <c r="AL23" s="45"/>
+      <c r="AM23" s="45"/>
+      <c r="AN23" s="45"/>
+      <c r="AO23" s="46"/>
+      <c r="AP23" s="44"/>
+      <c r="AQ23" s="45"/>
+      <c r="AR23" s="73"/>
     </row>
     <row r="24" spans="2:60" ht="9.9499999999999993" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="11"/>
@@ -3261,110 +3261,110 @@
       <c r="AR24" s="12"/>
     </row>
     <row r="25" spans="2:60" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="135" t="s">
+      <c r="B25" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="136"/>
-      <c r="D25" s="44" t="s">
+      <c r="C25" s="55"/>
+      <c r="D25" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="139" t="s">
+      <c r="E25" s="76"/>
+      <c r="F25" s="76"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="I25" s="140"/>
-      <c r="J25" s="140"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="141"/>
-      <c r="M25" s="44" t="s">
+      <c r="I25" s="79"/>
+      <c r="J25" s="79"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="27"/>
-      <c r="V25" s="139" t="s">
+      <c r="N25" s="76"/>
+      <c r="O25" s="76"/>
+      <c r="P25" s="76"/>
+      <c r="Q25" s="76"/>
+      <c r="R25" s="76"/>
+      <c r="S25" s="76"/>
+      <c r="T25" s="76"/>
+      <c r="U25" s="77"/>
+      <c r="V25" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="W25" s="140"/>
-      <c r="X25" s="140"/>
-      <c r="Y25" s="140"/>
-      <c r="Z25" s="140"/>
-      <c r="AA25" s="140"/>
-      <c r="AB25" s="140"/>
-      <c r="AC25" s="140"/>
-      <c r="AD25" s="140"/>
-      <c r="AE25" s="140"/>
-      <c r="AF25" s="141"/>
-      <c r="AG25" s="44" t="s">
+      <c r="W25" s="79"/>
+      <c r="X25" s="79"/>
+      <c r="Y25" s="79"/>
+      <c r="Z25" s="79"/>
+      <c r="AA25" s="79"/>
+      <c r="AB25" s="79"/>
+      <c r="AC25" s="79"/>
+      <c r="AD25" s="79"/>
+      <c r="AE25" s="79"/>
+      <c r="AF25" s="80"/>
+      <c r="AG25" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="AH25" s="26"/>
-      <c r="AI25" s="26"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="27"/>
-      <c r="AM25" s="44" t="s">
+      <c r="AH25" s="76"/>
+      <c r="AI25" s="76"/>
+      <c r="AJ25" s="76"/>
+      <c r="AK25" s="76"/>
+      <c r="AL25" s="77"/>
+      <c r="AM25" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="AN25" s="26"/>
-      <c r="AO25" s="26"/>
-      <c r="AP25" s="26"/>
-      <c r="AQ25" s="26"/>
-      <c r="AR25" s="45"/>
+      <c r="AN25" s="76"/>
+      <c r="AO25" s="76"/>
+      <c r="AP25" s="76"/>
+      <c r="AQ25" s="76"/>
+      <c r="AR25" s="81"/>
     </row>
     <row r="26" spans="2:60" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="137"/>
-      <c r="C26" s="138"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="102"/>
-      <c r="F26" s="102"/>
-      <c r="G26" s="103"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="102"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="101" t="s">
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="N26" s="102"/>
-      <c r="O26" s="102"/>
-      <c r="P26" s="102"/>
-      <c r="Q26" s="102"/>
-      <c r="R26" s="102"/>
-      <c r="S26" s="102"/>
-      <c r="T26" s="102"/>
-      <c r="U26" s="103"/>
-      <c r="V26" s="151"/>
-      <c r="W26" s="152"/>
-      <c r="X26" s="152"/>
-      <c r="Y26" s="152"/>
-      <c r="Z26" s="152"/>
-      <c r="AA26" s="152"/>
-      <c r="AB26" s="152"/>
-      <c r="AC26" s="152"/>
-      <c r="AD26" s="152"/>
-      <c r="AE26" s="152"/>
-      <c r="AF26" s="153"/>
-      <c r="AG26" s="101"/>
-      <c r="AH26" s="102"/>
-      <c r="AI26" s="102"/>
-      <c r="AJ26" s="102"/>
-      <c r="AK26" s="102"/>
-      <c r="AL26" s="103"/>
-      <c r="AM26" s="101"/>
-      <c r="AN26" s="102"/>
-      <c r="AO26" s="102"/>
-      <c r="AP26" s="102"/>
-      <c r="AQ26" s="102"/>
-      <c r="AR26" s="104"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="70"/>
+      <c r="W26" s="71"/>
+      <c r="X26" s="71"/>
+      <c r="Y26" s="71"/>
+      <c r="Z26" s="71"/>
+      <c r="AA26" s="71"/>
+      <c r="AB26" s="71"/>
+      <c r="AC26" s="71"/>
+      <c r="AD26" s="71"/>
+      <c r="AE26" s="71"/>
+      <c r="AF26" s="72"/>
+      <c r="AG26" s="44"/>
+      <c r="AH26" s="45"/>
+      <c r="AI26" s="45"/>
+      <c r="AJ26" s="45"/>
+      <c r="AK26" s="45"/>
+      <c r="AL26" s="46"/>
+      <c r="AM26" s="44"/>
+      <c r="AN26" s="45"/>
+      <c r="AO26" s="45"/>
+      <c r="AP26" s="45"/>
+      <c r="AQ26" s="45"/>
+      <c r="AR26" s="73"/>
     </row>
     <row r="27" spans="2:60" ht="9.9499999999999993" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="9"/>
@@ -3412,270 +3412,270 @@
       <c r="AR27" s="9"/>
     </row>
     <row r="28" spans="2:60" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="135" t="s">
+      <c r="B28" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="136"/>
-      <c r="D28" s="166" t="s">
+      <c r="C28" s="55"/>
+      <c r="D28" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="167"/>
-      <c r="F28" s="167"/>
-      <c r="G28" s="167"/>
-      <c r="H28" s="167"/>
-      <c r="I28" s="167"/>
-      <c r="J28" s="167"/>
-      <c r="K28" s="168"/>
-      <c r="L28" s="154" t="s">
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="M28" s="155"/>
-      <c r="N28" s="155"/>
-      <c r="O28" s="155"/>
-      <c r="P28" s="155"/>
-      <c r="Q28" s="155"/>
-      <c r="R28" s="155"/>
-      <c r="S28" s="155"/>
-      <c r="T28" s="155"/>
-      <c r="U28" s="169"/>
-      <c r="V28" s="170" t="s">
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="64"/>
+      <c r="Q28" s="64"/>
+      <c r="R28" s="64"/>
+      <c r="S28" s="64"/>
+      <c r="T28" s="64"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="W28" s="136"/>
-      <c r="X28" s="154" t="s">
+      <c r="W28" s="55"/>
+      <c r="X28" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="Y28" s="155"/>
-      <c r="Z28" s="155"/>
-      <c r="AA28" s="155"/>
-      <c r="AB28" s="155"/>
-      <c r="AC28" s="155"/>
-      <c r="AD28" s="155"/>
-      <c r="AE28" s="155"/>
-      <c r="AF28" s="169"/>
-      <c r="AG28" s="154" t="s">
+      <c r="Y28" s="64"/>
+      <c r="Z28" s="64"/>
+      <c r="AA28" s="64"/>
+      <c r="AB28" s="64"/>
+      <c r="AC28" s="64"/>
+      <c r="AD28" s="64"/>
+      <c r="AE28" s="64"/>
+      <c r="AF28" s="65"/>
+      <c r="AG28" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="AH28" s="155"/>
-      <c r="AI28" s="155"/>
-      <c r="AJ28" s="169"/>
-      <c r="AK28" s="154" t="s">
+      <c r="AH28" s="64"/>
+      <c r="AI28" s="64"/>
+      <c r="AJ28" s="65"/>
+      <c r="AK28" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="AL28" s="155"/>
-      <c r="AM28" s="155"/>
-      <c r="AN28" s="155"/>
-      <c r="AO28" s="155"/>
-      <c r="AP28" s="155"/>
-      <c r="AQ28" s="155"/>
-      <c r="AR28" s="156"/>
+      <c r="AL28" s="64"/>
+      <c r="AM28" s="64"/>
+      <c r="AN28" s="64"/>
+      <c r="AO28" s="64"/>
+      <c r="AP28" s="64"/>
+      <c r="AQ28" s="64"/>
+      <c r="AR28" s="74"/>
     </row>
     <row r="29" spans="2:60" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="164"/>
-      <c r="C29" s="165"/>
-      <c r="D29" s="157" t="s">
+      <c r="B29" s="56"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="158"/>
-      <c r="F29" s="158"/>
-      <c r="G29" s="158"/>
-      <c r="H29" s="158"/>
-      <c r="I29" s="158"/>
-      <c r="J29" s="158"/>
-      <c r="K29" s="159"/>
-      <c r="L29" s="91" t="s">
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92"/>
-      <c r="O29" s="92"/>
-      <c r="P29" s="92"/>
-      <c r="Q29" s="92"/>
-      <c r="R29" s="92"/>
-      <c r="S29" s="92"/>
-      <c r="T29" s="92"/>
-      <c r="U29" s="93"/>
-      <c r="V29" s="171"/>
-      <c r="W29" s="165"/>
-      <c r="X29" s="160"/>
-      <c r="Y29" s="161"/>
-      <c r="Z29" s="161"/>
-      <c r="AA29" s="161"/>
-      <c r="AB29" s="161"/>
-      <c r="AC29" s="161"/>
-      <c r="AD29" s="161"/>
-      <c r="AE29" s="161"/>
-      <c r="AF29" s="162"/>
-      <c r="AG29" s="160"/>
-      <c r="AH29" s="161"/>
-      <c r="AI29" s="161"/>
-      <c r="AJ29" s="162"/>
-      <c r="AK29" s="160"/>
-      <c r="AL29" s="161"/>
-      <c r="AM29" s="161"/>
-      <c r="AN29" s="161"/>
-      <c r="AO29" s="161"/>
-      <c r="AP29" s="161"/>
-      <c r="AQ29" s="161"/>
-      <c r="AR29" s="163"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="67"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="30"/>
+      <c r="Z29" s="30"/>
+      <c r="AA29" s="30"/>
+      <c r="AB29" s="30"/>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="30"/>
+      <c r="AE29" s="30"/>
+      <c r="AF29" s="53"/>
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="30"/>
+      <c r="AI29" s="30"/>
+      <c r="AJ29" s="53"/>
+      <c r="AK29" s="29"/>
+      <c r="AL29" s="30"/>
+      <c r="AM29" s="30"/>
+      <c r="AN29" s="30"/>
+      <c r="AO29" s="30"/>
+      <c r="AP29" s="30"/>
+      <c r="AQ29" s="30"/>
+      <c r="AR29" s="31"/>
     </row>
     <row r="30" spans="2:60" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="164"/>
-      <c r="C30" s="165"/>
-      <c r="D30" s="157" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="158"/>
-      <c r="J30" s="158"/>
-      <c r="K30" s="159"/>
-      <c r="L30" s="91" t="s">
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="M30" s="92"/>
-      <c r="N30" s="92"/>
-      <c r="O30" s="92"/>
-      <c r="P30" s="92"/>
-      <c r="Q30" s="92"/>
-      <c r="R30" s="92"/>
-      <c r="S30" s="92"/>
-      <c r="T30" s="92"/>
-      <c r="U30" s="93"/>
-      <c r="V30" s="172"/>
-      <c r="W30" s="173"/>
-      <c r="X30" s="160"/>
-      <c r="Y30" s="161"/>
-      <c r="Z30" s="161"/>
-      <c r="AA30" s="161"/>
-      <c r="AB30" s="161"/>
-      <c r="AC30" s="161"/>
-      <c r="AD30" s="161"/>
-      <c r="AE30" s="161"/>
-      <c r="AF30" s="162"/>
-      <c r="AG30" s="160"/>
-      <c r="AH30" s="161"/>
-      <c r="AI30" s="161"/>
-      <c r="AJ30" s="162"/>
-      <c r="AK30" s="160"/>
-      <c r="AL30" s="161"/>
-      <c r="AM30" s="161"/>
-      <c r="AN30" s="161"/>
-      <c r="AO30" s="161"/>
-      <c r="AP30" s="161"/>
-      <c r="AQ30" s="161"/>
-      <c r="AR30" s="163"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="68"/>
+      <c r="W30" s="69"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="30"/>
+      <c r="Z30" s="30"/>
+      <c r="AA30" s="30"/>
+      <c r="AB30" s="30"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="30"/>
+      <c r="AE30" s="30"/>
+      <c r="AF30" s="53"/>
+      <c r="AG30" s="29"/>
+      <c r="AH30" s="30"/>
+      <c r="AI30" s="30"/>
+      <c r="AJ30" s="53"/>
+      <c r="AK30" s="29"/>
+      <c r="AL30" s="30"/>
+      <c r="AM30" s="30"/>
+      <c r="AN30" s="30"/>
+      <c r="AO30" s="30"/>
+      <c r="AP30" s="30"/>
+      <c r="AQ30" s="30"/>
+      <c r="AR30" s="31"/>
     </row>
     <row r="31" spans="2:60" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="164"/>
-      <c r="C31" s="165"/>
-      <c r="D31" s="157" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="I31" s="158"/>
-      <c r="J31" s="158"/>
-      <c r="K31" s="159"/>
-      <c r="L31" s="91" t="s">
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="M31" s="92"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="92"/>
-      <c r="P31" s="92"/>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="92"/>
-      <c r="S31" s="92"/>
-      <c r="T31" s="92"/>
-      <c r="U31" s="93"/>
-      <c r="V31" s="84" t="s">
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="W31" s="85"/>
-      <c r="X31" s="85"/>
-      <c r="Y31" s="85"/>
-      <c r="Z31" s="85"/>
-      <c r="AA31" s="85"/>
-      <c r="AB31" s="85"/>
-      <c r="AC31" s="85"/>
-      <c r="AD31" s="85"/>
-      <c r="AE31" s="85"/>
-      <c r="AF31" s="86"/>
-      <c r="AG31" s="160" t="s">
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="39"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="39"/>
+      <c r="AB31" s="39"/>
+      <c r="AC31" s="39"/>
+      <c r="AD31" s="39"/>
+      <c r="AE31" s="39"/>
+      <c r="AF31" s="40"/>
+      <c r="AG31" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="AH31" s="161"/>
-      <c r="AI31" s="161"/>
-      <c r="AJ31" s="161"/>
-      <c r="AK31" s="161"/>
-      <c r="AL31" s="161"/>
-      <c r="AM31" s="161"/>
-      <c r="AN31" s="161"/>
-      <c r="AO31" s="161"/>
-      <c r="AP31" s="161"/>
-      <c r="AQ31" s="161"/>
-      <c r="AR31" s="163"/>
+      <c r="AH31" s="30"/>
+      <c r="AI31" s="30"/>
+      <c r="AJ31" s="30"/>
+      <c r="AK31" s="30"/>
+      <c r="AL31" s="30"/>
+      <c r="AM31" s="30"/>
+      <c r="AN31" s="30"/>
+      <c r="AO31" s="30"/>
+      <c r="AP31" s="30"/>
+      <c r="AQ31" s="30"/>
+      <c r="AR31" s="31"/>
       <c r="BH31" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="2:60" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="137"/>
-      <c r="C32" s="138"/>
-      <c r="D32" s="179" t="s">
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="180"/>
-      <c r="F32" s="180"/>
-      <c r="G32" s="180"/>
-      <c r="H32" s="180"/>
-      <c r="I32" s="180"/>
-      <c r="J32" s="180"/>
-      <c r="K32" s="181"/>
-      <c r="L32" s="101" t="s">
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="M32" s="102"/>
-      <c r="N32" s="102"/>
-      <c r="O32" s="102"/>
-      <c r="P32" s="102"/>
-      <c r="Q32" s="102"/>
-      <c r="R32" s="102"/>
-      <c r="S32" s="102"/>
-      <c r="T32" s="102"/>
-      <c r="U32" s="103"/>
-      <c r="V32" s="182" t="s">
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="W32" s="109"/>
-      <c r="X32" s="109"/>
-      <c r="Y32" s="109"/>
-      <c r="Z32" s="109"/>
-      <c r="AA32" s="109"/>
-      <c r="AB32" s="109"/>
-      <c r="AC32" s="109"/>
-      <c r="AD32" s="109"/>
-      <c r="AE32" s="109"/>
-      <c r="AF32" s="110"/>
-      <c r="AG32" s="183" t="s">
+      <c r="W32" s="48"/>
+      <c r="X32" s="48"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="48"/>
+      <c r="AA32" s="48"/>
+      <c r="AB32" s="48"/>
+      <c r="AC32" s="48"/>
+      <c r="AD32" s="48"/>
+      <c r="AE32" s="48"/>
+      <c r="AF32" s="49"/>
+      <c r="AG32" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="AH32" s="184"/>
-      <c r="AI32" s="184"/>
-      <c r="AJ32" s="184"/>
-      <c r="AK32" s="184"/>
-      <c r="AL32" s="184"/>
-      <c r="AM32" s="184"/>
-      <c r="AN32" s="184"/>
-      <c r="AO32" s="184"/>
-      <c r="AP32" s="184"/>
-      <c r="AQ32" s="184"/>
-      <c r="AR32" s="185"/>
+      <c r="AH32" s="51"/>
+      <c r="AI32" s="51"/>
+      <c r="AJ32" s="51"/>
+      <c r="AK32" s="51"/>
+      <c r="AL32" s="51"/>
+      <c r="AM32" s="51"/>
+      <c r="AN32" s="51"/>
+      <c r="AO32" s="51"/>
+      <c r="AP32" s="51"/>
+      <c r="AQ32" s="51"/>
+      <c r="AR32" s="52"/>
     </row>
     <row r="33" spans="2:81" ht="9.9499999999999993" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B33" s="15"/>
@@ -3925,51 +3925,51 @@
       <c r="AY37" s="21"/>
     </row>
     <row r="38" spans="2:81" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="176" t="s">
+      <c r="B38" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
-      <c r="G38" s="176"/>
-      <c r="H38" s="176"/>
-      <c r="I38" s="176"/>
-      <c r="J38" s="176"/>
-      <c r="K38" s="176"/>
-      <c r="L38" s="176"/>
-      <c r="M38" s="176"/>
-      <c r="N38" s="176"/>
-      <c r="O38" s="176"/>
-      <c r="P38" s="176"/>
-      <c r="Q38" s="176"/>
-      <c r="R38" s="176"/>
-      <c r="S38" s="176"/>
-      <c r="T38" s="176"/>
-      <c r="U38" s="176"/>
-      <c r="V38" s="176"/>
-      <c r="W38" s="176"/>
-      <c r="X38" s="176"/>
-      <c r="Y38" s="176"/>
-      <c r="Z38" s="176"/>
-      <c r="AA38" s="176"/>
-      <c r="AB38" s="176"/>
-      <c r="AC38" s="176"/>
-      <c r="AD38" s="176"/>
-      <c r="AE38" s="176"/>
-      <c r="AF38" s="176"/>
-      <c r="AG38" s="176"/>
-      <c r="AH38" s="176"/>
-      <c r="AI38" s="176"/>
-      <c r="AJ38" s="176"/>
-      <c r="AK38" s="176"/>
-      <c r="AL38" s="176"/>
-      <c r="AM38" s="176"/>
-      <c r="AN38" s="176"/>
-      <c r="AO38" s="176"/>
-      <c r="AP38" s="176"/>
-      <c r="AQ38" s="176"/>
-      <c r="AR38" s="176"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="26"/>
+      <c r="X38" s="26"/>
+      <c r="Y38" s="26"/>
+      <c r="Z38" s="26"/>
+      <c r="AA38" s="26"/>
+      <c r="AB38" s="26"/>
+      <c r="AC38" s="26"/>
+      <c r="AD38" s="26"/>
+      <c r="AE38" s="26"/>
+      <c r="AF38" s="26"/>
+      <c r="AG38" s="26"/>
+      <c r="AH38" s="26"/>
+      <c r="AI38" s="26"/>
+      <c r="AJ38" s="26"/>
+      <c r="AK38" s="26"/>
+      <c r="AL38" s="26"/>
+      <c r="AM38" s="26"/>
+      <c r="AN38" s="26"/>
+      <c r="AO38" s="26"/>
+      <c r="AP38" s="26"/>
+      <c r="AQ38" s="26"/>
+      <c r="AR38" s="26"/>
       <c r="AS38" s="21"/>
       <c r="AT38" s="21"/>
       <c r="AU38" s="21"/>
@@ -3979,51 +3979,51 @@
       <c r="AY38" s="21"/>
     </row>
     <row r="39" spans="2:81" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="177" t="s">
+      <c r="B39" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="177"/>
-      <c r="D39" s="177"/>
-      <c r="E39" s="177"/>
-      <c r="F39" s="177"/>
-      <c r="G39" s="177"/>
-      <c r="H39" s="177"/>
-      <c r="I39" s="177"/>
-      <c r="J39" s="177"/>
-      <c r="K39" s="177"/>
-      <c r="L39" s="177"/>
-      <c r="M39" s="177"/>
-      <c r="N39" s="177"/>
-      <c r="O39" s="177"/>
-      <c r="P39" s="177"/>
-      <c r="Q39" s="177"/>
-      <c r="R39" s="177"/>
-      <c r="S39" s="177"/>
-      <c r="T39" s="177"/>
-      <c r="U39" s="177"/>
-      <c r="V39" s="177"/>
-      <c r="W39" s="177"/>
-      <c r="X39" s="177"/>
-      <c r="Y39" s="177"/>
-      <c r="Z39" s="177"/>
-      <c r="AA39" s="177"/>
-      <c r="AB39" s="177"/>
-      <c r="AC39" s="177"/>
-      <c r="AD39" s="177"/>
-      <c r="AE39" s="177"/>
-      <c r="AF39" s="177"/>
-      <c r="AG39" s="177"/>
-      <c r="AH39" s="177"/>
-      <c r="AI39" s="177"/>
-      <c r="AJ39" s="177"/>
-      <c r="AK39" s="177"/>
-      <c r="AL39" s="177"/>
-      <c r="AM39" s="177"/>
-      <c r="AN39" s="177"/>
-      <c r="AO39" s="177"/>
-      <c r="AP39" s="177"/>
-      <c r="AQ39" s="177"/>
-      <c r="AR39" s="177"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27"/>
+      <c r="W39" s="27"/>
+      <c r="X39" s="27"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="27"/>
+      <c r="AC39" s="27"/>
+      <c r="AD39" s="27"/>
+      <c r="AE39" s="27"/>
+      <c r="AF39" s="27"/>
+      <c r="AG39" s="27"/>
+      <c r="AH39" s="27"/>
+      <c r="AI39" s="27"/>
+      <c r="AJ39" s="27"/>
+      <c r="AK39" s="27"/>
+      <c r="AL39" s="27"/>
+      <c r="AM39" s="27"/>
+      <c r="AN39" s="27"/>
+      <c r="AO39" s="27"/>
+      <c r="AP39" s="27"/>
+      <c r="AQ39" s="27"/>
+      <c r="AR39" s="27"/>
       <c r="AS39" s="21"/>
       <c r="AT39" s="21"/>
       <c r="AU39" s="21"/>
@@ -4033,51 +4033,51 @@
       <c r="AY39" s="21"/>
     </row>
     <row r="40" spans="2:81" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="176" t="s">
+      <c r="B40" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="176"/>
-      <c r="D40" s="176"/>
-      <c r="E40" s="176"/>
-      <c r="F40" s="176"/>
-      <c r="G40" s="176"/>
-      <c r="H40" s="176"/>
-      <c r="I40" s="176"/>
-      <c r="J40" s="176"/>
-      <c r="K40" s="176"/>
-      <c r="L40" s="176"/>
-      <c r="M40" s="176"/>
-      <c r="N40" s="176"/>
-      <c r="O40" s="176"/>
-      <c r="P40" s="176"/>
-      <c r="Q40" s="176"/>
-      <c r="R40" s="176"/>
-      <c r="S40" s="176"/>
-      <c r="T40" s="176"/>
-      <c r="U40" s="176"/>
-      <c r="V40" s="176"/>
-      <c r="W40" s="176"/>
-      <c r="X40" s="176"/>
-      <c r="Y40" s="176"/>
-      <c r="Z40" s="176"/>
-      <c r="AA40" s="176"/>
-      <c r="AB40" s="176"/>
-      <c r="AC40" s="176"/>
-      <c r="AD40" s="176"/>
-      <c r="AE40" s="176"/>
-      <c r="AF40" s="176"/>
-      <c r="AG40" s="176"/>
-      <c r="AH40" s="176"/>
-      <c r="AI40" s="176"/>
-      <c r="AJ40" s="176"/>
-      <c r="AK40" s="176"/>
-      <c r="AL40" s="176"/>
-      <c r="AM40" s="176"/>
-      <c r="AN40" s="176"/>
-      <c r="AO40" s="176"/>
-      <c r="AP40" s="176"/>
-      <c r="AQ40" s="176"/>
-      <c r="AR40" s="176"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="26"/>
+      <c r="AD40" s="26"/>
+      <c r="AE40" s="26"/>
+      <c r="AF40" s="26"/>
+      <c r="AG40" s="26"/>
+      <c r="AH40" s="26"/>
+      <c r="AI40" s="26"/>
+      <c r="AJ40" s="26"/>
+      <c r="AK40" s="26"/>
+      <c r="AL40" s="26"/>
+      <c r="AM40" s="26"/>
+      <c r="AN40" s="26"/>
+      <c r="AO40" s="26"/>
+      <c r="AP40" s="26"/>
+      <c r="AQ40" s="26"/>
+      <c r="AR40" s="26"/>
       <c r="AS40" s="21"/>
       <c r="AT40" s="21"/>
       <c r="AU40" s="21"/>
@@ -4087,38 +4087,38 @@
       <c r="AY40" s="21"/>
     </row>
     <row r="41" spans="2:81" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="176" t="s">
+      <c r="B41" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="176"/>
-      <c r="D41" s="176"/>
-      <c r="E41" s="176"/>
-      <c r="F41" s="176"/>
-      <c r="G41" s="176"/>
-      <c r="H41" s="176"/>
-      <c r="I41" s="176"/>
-      <c r="J41" s="176"/>
-      <c r="K41" s="176"/>
-      <c r="L41" s="176"/>
-      <c r="M41" s="176"/>
-      <c r="N41" s="176"/>
-      <c r="O41" s="176"/>
-      <c r="P41" s="176"/>
-      <c r="Q41" s="176"/>
-      <c r="R41" s="176"/>
-      <c r="S41" s="176"/>
-      <c r="T41" s="176"/>
-      <c r="U41" s="176"/>
-      <c r="V41" s="176"/>
-      <c r="W41" s="176"/>
-      <c r="X41" s="176"/>
-      <c r="Y41" s="176"/>
-      <c r="Z41" s="176"/>
-      <c r="AA41" s="176"/>
-      <c r="AB41" s="176"/>
-      <c r="AC41" s="176"/>
-      <c r="AD41" s="176"/>
-      <c r="AE41" s="176"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="26"/>
+      <c r="AD41" s="26"/>
+      <c r="AE41" s="26"/>
       <c r="AF41" s="22"/>
       <c r="AG41" s="22"/>
       <c r="AH41" s="22"/>
@@ -4245,51 +4245,51 @@
       <c r="AY43" s="21"/>
     </row>
     <row r="44" spans="2:81" s="9" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="175" t="s">
+      <c r="B44" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="175"/>
-      <c r="D44" s="175"/>
-      <c r="E44" s="175"/>
-      <c r="F44" s="175"/>
-      <c r="G44" s="175"/>
-      <c r="H44" s="175"/>
-      <c r="I44" s="175"/>
-      <c r="J44" s="175"/>
-      <c r="K44" s="175"/>
-      <c r="L44" s="175"/>
-      <c r="M44" s="175"/>
-      <c r="N44" s="175"/>
-      <c r="O44" s="175"/>
-      <c r="P44" s="175"/>
-      <c r="Q44" s="175"/>
-      <c r="R44" s="175"/>
-      <c r="S44" s="175"/>
-      <c r="T44" s="175"/>
-      <c r="U44" s="175"/>
-      <c r="V44" s="175"/>
-      <c r="W44" s="175"/>
-      <c r="X44" s="175"/>
-      <c r="Y44" s="175"/>
-      <c r="Z44" s="175"/>
-      <c r="AA44" s="175"/>
-      <c r="AB44" s="175"/>
-      <c r="AC44" s="175"/>
-      <c r="AD44" s="175"/>
-      <c r="AE44" s="175"/>
-      <c r="AF44" s="175"/>
-      <c r="AG44" s="175"/>
-      <c r="AH44" s="175"/>
-      <c r="AI44" s="175"/>
-      <c r="AJ44" s="175"/>
-      <c r="AK44" s="175"/>
-      <c r="AL44" s="175"/>
-      <c r="AM44" s="175"/>
-      <c r="AN44" s="175"/>
-      <c r="AO44" s="175"/>
-      <c r="AP44" s="175"/>
-      <c r="AQ44" s="175"/>
-      <c r="AR44" s="175"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25"/>
+      <c r="T44" s="25"/>
+      <c r="U44" s="25"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="25"/>
+      <c r="X44" s="25"/>
+      <c r="Y44" s="25"/>
+      <c r="Z44" s="25"/>
+      <c r="AA44" s="25"/>
+      <c r="AB44" s="25"/>
+      <c r="AC44" s="25"/>
+      <c r="AD44" s="25"/>
+      <c r="AE44" s="25"/>
+      <c r="AF44" s="25"/>
+      <c r="AG44" s="25"/>
+      <c r="AH44" s="25"/>
+      <c r="AI44" s="25"/>
+      <c r="AJ44" s="25"/>
+      <c r="AK44" s="25"/>
+      <c r="AL44" s="25"/>
+      <c r="AM44" s="25"/>
+      <c r="AN44" s="25"/>
+      <c r="AO44" s="25"/>
+      <c r="AP44" s="25"/>
+      <c r="AQ44" s="25"/>
+      <c r="AR44" s="25"/>
       <c r="AS44" s="23"/>
       <c r="AT44" s="23"/>
       <c r="AU44" s="23"/>
@@ -4299,120 +4299,138 @@
       <c r="AY44" s="23"/>
     </row>
     <row r="45" spans="2:81" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="178" t="s">
+      <c r="B45" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="178"/>
-      <c r="D45" s="178"/>
-      <c r="E45" s="178"/>
-      <c r="F45" s="178"/>
-      <c r="G45" s="178"/>
-      <c r="H45" s="178"/>
-      <c r="I45" s="178"/>
-      <c r="J45" s="178"/>
-      <c r="K45" s="178"/>
-      <c r="L45" s="178"/>
-      <c r="M45" s="178"/>
-      <c r="N45" s="178"/>
-      <c r="O45" s="178"/>
-      <c r="P45" s="178"/>
-      <c r="Q45" s="178"/>
-      <c r="R45" s="178"/>
-      <c r="S45" s="178"/>
-      <c r="T45" s="178"/>
-      <c r="U45" s="178"/>
-      <c r="V45" s="178"/>
-      <c r="W45" s="178"/>
-      <c r="X45" s="178"/>
-      <c r="Y45" s="178"/>
-      <c r="Z45" s="178"/>
-      <c r="AA45" s="178"/>
-      <c r="AB45" s="178"/>
-      <c r="AC45" s="178"/>
-      <c r="AD45" s="178"/>
-      <c r="AE45" s="178"/>
-      <c r="AF45" s="178"/>
-      <c r="AG45" s="178"/>
-      <c r="AH45" s="178"/>
-      <c r="AI45" s="178"/>
-      <c r="AJ45" s="178"/>
-      <c r="AK45" s="178"/>
-      <c r="AL45" s="178"/>
-      <c r="AM45" s="178"/>
-      <c r="AN45" s="178"/>
-      <c r="AO45" s="178"/>
-      <c r="AP45" s="178"/>
-      <c r="AQ45" s="178"/>
-      <c r="AR45" s="178"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="T45" s="28"/>
+      <c r="U45" s="28"/>
+      <c r="V45" s="28"/>
+      <c r="W45" s="28"/>
+      <c r="X45" s="28"/>
+      <c r="Y45" s="28"/>
+      <c r="Z45" s="28"/>
+      <c r="AA45" s="28"/>
+      <c r="AB45" s="28"/>
+      <c r="AC45" s="28"/>
+      <c r="AD45" s="28"/>
+      <c r="AE45" s="28"/>
+      <c r="AF45" s="28"/>
+      <c r="AG45" s="28"/>
+      <c r="AH45" s="28"/>
+      <c r="AI45" s="28"/>
+      <c r="AJ45" s="28"/>
+      <c r="AK45" s="28"/>
+      <c r="AL45" s="28"/>
+      <c r="AM45" s="28"/>
+      <c r="AN45" s="28"/>
+      <c r="AO45" s="28"/>
+      <c r="AP45" s="28"/>
+      <c r="AQ45" s="28"/>
+      <c r="AR45" s="28"/>
       <c r="CC45" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="47" spans="2:81" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AB47" s="174"/>
-      <c r="AC47" s="174"/>
-      <c r="AD47" s="174"/>
-      <c r="AE47" s="174"/>
-      <c r="AF47" s="174"/>
-      <c r="AG47" s="174"/>
-      <c r="AH47" s="174"/>
-      <c r="AI47" s="175"/>
-      <c r="AJ47" s="175"/>
-      <c r="AK47" s="175"/>
-      <c r="AL47" s="175"/>
-      <c r="AM47" s="175"/>
-      <c r="AN47" s="175"/>
-      <c r="AO47" s="175"/>
-      <c r="AP47" s="175"/>
-      <c r="AQ47" s="175"/>
-      <c r="AR47" s="175"/>
-      <c r="AS47" s="175"/>
-      <c r="AT47" s="175"/>
-      <c r="AU47" s="175"/>
+      <c r="AB47" s="24"/>
+      <c r="AC47" s="24"/>
+      <c r="AD47" s="24"/>
+      <c r="AE47" s="24"/>
+      <c r="AF47" s="24"/>
+      <c r="AG47" s="24"/>
+      <c r="AH47" s="24"/>
+      <c r="AI47" s="25"/>
+      <c r="AJ47" s="25"/>
+      <c r="AK47" s="25"/>
+      <c r="AL47" s="25"/>
+      <c r="AM47" s="25"/>
+      <c r="AN47" s="25"/>
+      <c r="AO47" s="25"/>
+      <c r="AP47" s="25"/>
+      <c r="AQ47" s="25"/>
+      <c r="AR47" s="25"/>
+      <c r="AS47" s="25"/>
+      <c r="AT47" s="25"/>
+      <c r="AU47" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="AB47:AH47"/>
-    <mergeCell ref="AI47:AU47"/>
-    <mergeCell ref="B38:AR38"/>
-    <mergeCell ref="B39:AR39"/>
-    <mergeCell ref="B40:AR40"/>
-    <mergeCell ref="B41:AE41"/>
-    <mergeCell ref="B44:AR44"/>
-    <mergeCell ref="B45:AR45"/>
-    <mergeCell ref="AK30:AR30"/>
-    <mergeCell ref="D31:K31"/>
-    <mergeCell ref="L31:U31"/>
-    <mergeCell ref="V31:AF31"/>
-    <mergeCell ref="AG31:AR31"/>
-    <mergeCell ref="D32:K32"/>
-    <mergeCell ref="L32:U32"/>
-    <mergeCell ref="V32:AF32"/>
-    <mergeCell ref="AG32:AR32"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="L29:U29"/>
-    <mergeCell ref="X29:AF29"/>
-    <mergeCell ref="AG29:AJ29"/>
-    <mergeCell ref="AK29:AR29"/>
-    <mergeCell ref="B28:C32"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="L28:U28"/>
-    <mergeCell ref="V28:W30"/>
-    <mergeCell ref="X28:AF28"/>
-    <mergeCell ref="AG28:AJ28"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="L30:U30"/>
-    <mergeCell ref="X30:AF30"/>
-    <mergeCell ref="AG30:AJ30"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="M26:U26"/>
-    <mergeCell ref="V26:AF26"/>
-    <mergeCell ref="AG26:AL26"/>
-    <mergeCell ref="AM26:AR26"/>
-    <mergeCell ref="AG23:AJ23"/>
-    <mergeCell ref="AK23:AO23"/>
-    <mergeCell ref="AP23:AR23"/>
-    <mergeCell ref="AK28:AR28"/>
+    <mergeCell ref="A1:AS1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="AC3:AR3"/>
+    <mergeCell ref="B10:C12"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O10:AB10"/>
+    <mergeCell ref="AC10:AJ10"/>
+    <mergeCell ref="AK10:AR10"/>
+    <mergeCell ref="D11:N11"/>
+    <mergeCell ref="B4:H8"/>
+    <mergeCell ref="I4:N5"/>
+    <mergeCell ref="O4:AB4"/>
+    <mergeCell ref="AC4:AF5"/>
+    <mergeCell ref="AG4:AR5"/>
+    <mergeCell ref="O5:AB5"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="O6:AB6"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="AG6:AR6"/>
+    <mergeCell ref="O11:AB11"/>
+    <mergeCell ref="AC11:AJ11"/>
+    <mergeCell ref="AK11:AR11"/>
+    <mergeCell ref="D12:N12"/>
+    <mergeCell ref="O12:AB12"/>
+    <mergeCell ref="AC12:AJ12"/>
+    <mergeCell ref="AK12:AR12"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="O7:AR7"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="O8:AR8"/>
+    <mergeCell ref="O16:AB16"/>
+    <mergeCell ref="AC16:AJ16"/>
+    <mergeCell ref="AK16:AR16"/>
+    <mergeCell ref="D17:N17"/>
+    <mergeCell ref="O17:AB17"/>
+    <mergeCell ref="AC17:AJ17"/>
+    <mergeCell ref="AK17:AR17"/>
+    <mergeCell ref="B14:C17"/>
+    <mergeCell ref="D14:N14"/>
+    <mergeCell ref="O14:AB14"/>
+    <mergeCell ref="AC14:AJ14"/>
+    <mergeCell ref="AK14:AR14"/>
+    <mergeCell ref="D15:N15"/>
+    <mergeCell ref="O15:AB15"/>
+    <mergeCell ref="AC15:AJ15"/>
+    <mergeCell ref="AK15:AR15"/>
+    <mergeCell ref="D16:N16"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="K19:U19"/>
+    <mergeCell ref="V19:AF19"/>
+    <mergeCell ref="AG19:AR19"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="K20:U20"/>
+    <mergeCell ref="V20:AF20"/>
+    <mergeCell ref="AG20:AR20"/>
     <mergeCell ref="B25:C26"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="H25:L25"/>
@@ -4437,65 +4455,47 @@
     <mergeCell ref="R22:AB22"/>
     <mergeCell ref="AC22:AF22"/>
     <mergeCell ref="D26:G26"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="K19:U19"/>
-    <mergeCell ref="V19:AF19"/>
-    <mergeCell ref="AG19:AR19"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="K20:U20"/>
-    <mergeCell ref="V20:AF20"/>
-    <mergeCell ref="AG20:AR20"/>
-    <mergeCell ref="O16:AB16"/>
-    <mergeCell ref="AC16:AJ16"/>
-    <mergeCell ref="AK16:AR16"/>
-    <mergeCell ref="D17:N17"/>
-    <mergeCell ref="O17:AB17"/>
-    <mergeCell ref="AC17:AJ17"/>
-    <mergeCell ref="AK17:AR17"/>
-    <mergeCell ref="B14:C17"/>
-    <mergeCell ref="D14:N14"/>
-    <mergeCell ref="O14:AB14"/>
-    <mergeCell ref="AC14:AJ14"/>
-    <mergeCell ref="AK14:AR14"/>
-    <mergeCell ref="D15:N15"/>
-    <mergeCell ref="O15:AB15"/>
-    <mergeCell ref="AC15:AJ15"/>
-    <mergeCell ref="AK15:AR15"/>
-    <mergeCell ref="D16:N16"/>
-    <mergeCell ref="AK11:AR11"/>
-    <mergeCell ref="D12:N12"/>
-    <mergeCell ref="O12:AB12"/>
-    <mergeCell ref="AC12:AJ12"/>
-    <mergeCell ref="AK12:AR12"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="O7:AR7"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="O8:AR8"/>
-    <mergeCell ref="A1:AS1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="AC3:AR3"/>
-    <mergeCell ref="B10:C12"/>
-    <mergeCell ref="D10:N10"/>
-    <mergeCell ref="O10:AB10"/>
-    <mergeCell ref="AC10:AJ10"/>
-    <mergeCell ref="AK10:AR10"/>
-    <mergeCell ref="D11:N11"/>
-    <mergeCell ref="B4:H8"/>
-    <mergeCell ref="I4:N5"/>
-    <mergeCell ref="O4:AB4"/>
-    <mergeCell ref="AC4:AF5"/>
-    <mergeCell ref="AG4:AR5"/>
-    <mergeCell ref="O5:AB5"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="O6:AB6"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="AG6:AR6"/>
-    <mergeCell ref="O11:AB11"/>
-    <mergeCell ref="AC11:AJ11"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="M26:U26"/>
+    <mergeCell ref="V26:AF26"/>
+    <mergeCell ref="AG26:AL26"/>
+    <mergeCell ref="AM26:AR26"/>
+    <mergeCell ref="AG23:AJ23"/>
+    <mergeCell ref="AK23:AO23"/>
+    <mergeCell ref="AP23:AR23"/>
+    <mergeCell ref="AK28:AR28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="L29:U29"/>
+    <mergeCell ref="X29:AF29"/>
+    <mergeCell ref="AG29:AJ29"/>
+    <mergeCell ref="AK29:AR29"/>
+    <mergeCell ref="B28:C32"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="L28:U28"/>
+    <mergeCell ref="V28:W30"/>
+    <mergeCell ref="X28:AF28"/>
+    <mergeCell ref="AG28:AJ28"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="L30:U30"/>
+    <mergeCell ref="X30:AF30"/>
+    <mergeCell ref="AG30:AJ30"/>
+    <mergeCell ref="AB47:AH47"/>
+    <mergeCell ref="AI47:AU47"/>
+    <mergeCell ref="B38:AR38"/>
+    <mergeCell ref="B39:AR39"/>
+    <mergeCell ref="B40:AR40"/>
+    <mergeCell ref="B41:AE41"/>
+    <mergeCell ref="B44:AR44"/>
+    <mergeCell ref="B45:AR45"/>
+    <mergeCell ref="AK30:AR30"/>
+    <mergeCell ref="D31:K31"/>
+    <mergeCell ref="L31:U31"/>
+    <mergeCell ref="V31:AF31"/>
+    <mergeCell ref="AG31:AR31"/>
+    <mergeCell ref="D32:K32"/>
+    <mergeCell ref="L32:U32"/>
+    <mergeCell ref="V32:AF32"/>
+    <mergeCell ref="AG32:AR32"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
refactor: Migrate Chat component to use `useChat` hook instead of `useChatStore`.
</commit_message>
<xml_diff>
--- a/templates/excel/입사지원서.xlsx
+++ b/templates/excel/입사지원서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d16d419a79d4019c/dev/Humetix_Project/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{D6DA580A-CC61-4BB7-B199-D8C038C296A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D13AB22B-3650-49DE-A01D-77A21BA64D24}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{D6DA580A-CC61-4BB7-B199-D8C038C296A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25DC8561-90ED-489E-BD16-456229F7BEF6}"/>
   <bookViews>
     <workbookView xWindow="28410" yWindow="0" windowWidth="25590" windowHeight="21000" xr2:uid="{5B50BEF5-311F-42AB-98EF-5572324690B7}"/>
   </bookViews>
@@ -406,24 +406,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(한글)      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> OOO</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>010-1234-5678</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -454,13 +436,17 @@
   <si>
     <t>주간 , 2교대</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>(한글)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,15 +572,6 @@
     <font>
       <b/>
       <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1089,7 +1066,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1136,16 +1113,16 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1157,7 +1134,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1454,13 +1431,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1583,15 +1560,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1625,16 +1593,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1645,6 +1613,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2041,8 +2021,8 @@
   </sheetPr>
   <dimension ref="A1:CC47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="BH14" sqref="BH14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="93" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10:AJ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2242,42 +2222,42 @@
       <c r="L4" s="160"/>
       <c r="M4" s="160"/>
       <c r="N4" s="161"/>
-      <c r="O4" s="165" t="s">
-        <v>90</v>
-      </c>
-      <c r="P4" s="166"/>
-      <c r="Q4" s="166"/>
-      <c r="R4" s="166"/>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
-      <c r="U4" s="166"/>
-      <c r="V4" s="166"/>
-      <c r="W4" s="166"/>
-      <c r="X4" s="166"/>
-      <c r="Y4" s="166"/>
-      <c r="Z4" s="166"/>
-      <c r="AA4" s="166"/>
-      <c r="AB4" s="167"/>
-      <c r="AC4" s="168" t="s">
+      <c r="O4" s="183" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="184"/>
+      <c r="Q4" s="184"/>
+      <c r="R4" s="185"/>
+      <c r="S4" s="185"/>
+      <c r="T4" s="185"/>
+      <c r="U4" s="185"/>
+      <c r="V4" s="185"/>
+      <c r="W4" s="185"/>
+      <c r="X4" s="185"/>
+      <c r="Y4" s="185"/>
+      <c r="Z4" s="185"/>
+      <c r="AA4" s="185"/>
+      <c r="AB4" s="186"/>
+      <c r="AC4" s="165" t="s">
         <v>4</v>
       </c>
       <c r="AD4" s="160"/>
       <c r="AE4" s="160"/>
       <c r="AF4" s="161"/>
-      <c r="AG4" s="170" t="s">
-        <v>92</v>
-      </c>
-      <c r="AH4" s="171"/>
-      <c r="AI4" s="171"/>
-      <c r="AJ4" s="171"/>
-      <c r="AK4" s="171"/>
-      <c r="AL4" s="171"/>
-      <c r="AM4" s="171"/>
-      <c r="AN4" s="171"/>
-      <c r="AO4" s="171"/>
-      <c r="AP4" s="171"/>
-      <c r="AQ4" s="171"/>
-      <c r="AR4" s="172"/>
+      <c r="AG4" s="167" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH4" s="168"/>
+      <c r="AI4" s="168"/>
+      <c r="AJ4" s="168"/>
+      <c r="AK4" s="168"/>
+      <c r="AL4" s="168"/>
+      <c r="AM4" s="168"/>
+      <c r="AN4" s="168"/>
+      <c r="AO4" s="168"/>
+      <c r="AP4" s="168"/>
+      <c r="AQ4" s="168"/>
+      <c r="AR4" s="169"/>
     </row>
     <row r="5" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="153"/>
@@ -2293,38 +2273,38 @@
       <c r="L5" s="163"/>
       <c r="M5" s="163"/>
       <c r="N5" s="164"/>
-      <c r="O5" s="176" t="s">
+      <c r="O5" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="177"/>
-      <c r="Q5" s="177"/>
-      <c r="R5" s="177"/>
-      <c r="S5" s="177"/>
-      <c r="T5" s="177"/>
-      <c r="U5" s="177"/>
-      <c r="V5" s="177"/>
-      <c r="W5" s="177"/>
-      <c r="X5" s="177"/>
-      <c r="Y5" s="177"/>
-      <c r="Z5" s="177"/>
-      <c r="AA5" s="177"/>
-      <c r="AB5" s="178"/>
-      <c r="AC5" s="169"/>
+      <c r="P5" s="174"/>
+      <c r="Q5" s="174"/>
+      <c r="R5" s="174"/>
+      <c r="S5" s="174"/>
+      <c r="T5" s="174"/>
+      <c r="U5" s="174"/>
+      <c r="V5" s="174"/>
+      <c r="W5" s="174"/>
+      <c r="X5" s="174"/>
+      <c r="Y5" s="174"/>
+      <c r="Z5" s="174"/>
+      <c r="AA5" s="174"/>
+      <c r="AB5" s="175"/>
+      <c r="AC5" s="166"/>
       <c r="AD5" s="163"/>
       <c r="AE5" s="163"/>
       <c r="AF5" s="164"/>
-      <c r="AG5" s="173"/>
-      <c r="AH5" s="174"/>
-      <c r="AI5" s="174"/>
-      <c r="AJ5" s="174"/>
-      <c r="AK5" s="174"/>
-      <c r="AL5" s="174"/>
-      <c r="AM5" s="174"/>
-      <c r="AN5" s="174"/>
-      <c r="AO5" s="174"/>
-      <c r="AP5" s="174"/>
-      <c r="AQ5" s="174"/>
-      <c r="AR5" s="175"/>
+      <c r="AG5" s="170"/>
+      <c r="AH5" s="171"/>
+      <c r="AI5" s="171"/>
+      <c r="AJ5" s="171"/>
+      <c r="AK5" s="171"/>
+      <c r="AL5" s="171"/>
+      <c r="AM5" s="171"/>
+      <c r="AN5" s="171"/>
+      <c r="AO5" s="171"/>
+      <c r="AP5" s="171"/>
+      <c r="AQ5" s="171"/>
+      <c r="AR5" s="172"/>
     </row>
     <row r="6" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="153"/>
@@ -2342,42 +2322,42 @@
       <c r="L6" s="120"/>
       <c r="M6" s="120"/>
       <c r="N6" s="121"/>
-      <c r="O6" s="179" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="180"/>
-      <c r="Q6" s="180"/>
-      <c r="R6" s="180"/>
-      <c r="S6" s="180"/>
-      <c r="T6" s="180"/>
-      <c r="U6" s="180"/>
-      <c r="V6" s="180"/>
-      <c r="W6" s="180"/>
-      <c r="X6" s="180"/>
-      <c r="Y6" s="180"/>
-      <c r="Z6" s="180"/>
-      <c r="AA6" s="180"/>
-      <c r="AB6" s="181"/>
+      <c r="O6" s="176" t="s">
+        <v>90</v>
+      </c>
+      <c r="P6" s="177"/>
+      <c r="Q6" s="177"/>
+      <c r="R6" s="177"/>
+      <c r="S6" s="177"/>
+      <c r="T6" s="177"/>
+      <c r="U6" s="177"/>
+      <c r="V6" s="177"/>
+      <c r="W6" s="177"/>
+      <c r="X6" s="177"/>
+      <c r="Y6" s="177"/>
+      <c r="Z6" s="177"/>
+      <c r="AA6" s="177"/>
+      <c r="AB6" s="178"/>
       <c r="AC6" s="38" t="s">
         <v>7</v>
       </c>
       <c r="AD6" s="39"/>
       <c r="AE6" s="39"/>
       <c r="AF6" s="40"/>
-      <c r="AG6" s="179" t="s">
+      <c r="AG6" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="AH6" s="180"/>
-      <c r="AI6" s="180"/>
-      <c r="AJ6" s="180"/>
-      <c r="AK6" s="180"/>
-      <c r="AL6" s="180"/>
-      <c r="AM6" s="180"/>
-      <c r="AN6" s="180"/>
-      <c r="AO6" s="180"/>
-      <c r="AP6" s="180"/>
-      <c r="AQ6" s="180"/>
-      <c r="AR6" s="182"/>
+      <c r="AH6" s="177"/>
+      <c r="AI6" s="177"/>
+      <c r="AJ6" s="177"/>
+      <c r="AK6" s="177"/>
+      <c r="AL6" s="177"/>
+      <c r="AM6" s="177"/>
+      <c r="AN6" s="177"/>
+      <c r="AO6" s="177"/>
+      <c r="AP6" s="177"/>
+      <c r="AQ6" s="177"/>
+      <c r="AR6" s="179"/>
     </row>
     <row r="7" spans="1:45" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="153"/>
@@ -2550,22 +2530,22 @@
       <c r="L11" s="148"/>
       <c r="M11" s="148"/>
       <c r="N11" s="149"/>
-      <c r="O11" s="183" t="s">
+      <c r="O11" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="184"/>
-      <c r="Q11" s="184"/>
-      <c r="R11" s="184"/>
-      <c r="S11" s="184"/>
-      <c r="T11" s="184"/>
-      <c r="U11" s="184"/>
-      <c r="V11" s="184"/>
-      <c r="W11" s="184"/>
-      <c r="X11" s="184"/>
-      <c r="Y11" s="184"/>
-      <c r="Z11" s="184"/>
-      <c r="AA11" s="184"/>
-      <c r="AB11" s="185"/>
+      <c r="P11" s="181"/>
+      <c r="Q11" s="181"/>
+      <c r="R11" s="181"/>
+      <c r="S11" s="181"/>
+      <c r="T11" s="181"/>
+      <c r="U11" s="181"/>
+      <c r="V11" s="181"/>
+      <c r="W11" s="181"/>
+      <c r="X11" s="181"/>
+      <c r="Y11" s="181"/>
+      <c r="Z11" s="181"/>
+      <c r="AA11" s="181"/>
+      <c r="AB11" s="182"/>
       <c r="AC11" s="35"/>
       <c r="AD11" s="36"/>
       <c r="AE11" s="36"/>
@@ -3427,7 +3407,7 @@
       <c r="J28" s="61"/>
       <c r="K28" s="62"/>
       <c r="L28" s="63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M28" s="64"/>
       <c r="N28" s="64"/>
@@ -3474,7 +3454,7 @@
       <c r="B29" s="56"/>
       <c r="C29" s="57"/>
       <c r="D29" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
@@ -3523,7 +3503,7 @@
       <c r="B30" s="56"/>
       <c r="C30" s="57"/>
       <c r="D30" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
@@ -3572,7 +3552,7 @@
       <c r="B31" s="56"/>
       <c r="C31" s="57"/>
       <c r="D31" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
@@ -3663,7 +3643,7 @@
       <c r="AE32" s="48"/>
       <c r="AF32" s="49"/>
       <c r="AG32" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AH32" s="51"/>
       <c r="AI32" s="51"/>
@@ -4246,7 +4226,7 @@
     </row>
     <row r="44" spans="2:81" s="9" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
@@ -4372,6 +4352,7 @@
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="R4:AB4"/>
     <mergeCell ref="A1:AS1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:K2"/>
@@ -4386,7 +4367,6 @@
     <mergeCell ref="D11:N11"/>
     <mergeCell ref="B4:H8"/>
     <mergeCell ref="I4:N5"/>
-    <mergeCell ref="O4:AB4"/>
     <mergeCell ref="AC4:AF5"/>
     <mergeCell ref="AG4:AR5"/>
     <mergeCell ref="O5:AB5"/>

</xml_diff>